<commit_message>
Communication AX12 (envoi et reception) fonctionelles Mapping carte V2 ajouté au projet, mais problème pour la pwm Y dont les schémas elec ne sont pas bons ...
</commit_message>
<xml_diff>
--- a/Excel reglages/Mapping carte stratV1.xlsx
+++ b/Excel reglages/Mapping carte stratV1.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28515" windowHeight="13095"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="28515" windowHeight="13095" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="Mapping Carte V1.0" sheetId="1" r:id="rId1"/>
+    <sheet name="Mapping Carte V2.0" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="116">
   <si>
     <t>RA0</t>
   </si>
@@ -307,13 +308,70 @@
   </si>
   <si>
     <t>AN1</t>
+  </si>
+  <si>
+    <t>XBEE RST</t>
+  </si>
+  <si>
+    <t>Couleur</t>
+  </si>
+  <si>
+    <t>sens Y</t>
+  </si>
+  <si>
+    <t>PWM Y</t>
+  </si>
+  <si>
+    <t>TX AX12</t>
+  </si>
+  <si>
+    <t>sens G</t>
+  </si>
+  <si>
+    <t>PWM G</t>
+  </si>
+  <si>
+    <t>sens D</t>
+  </si>
+  <si>
+    <t>PWM D</t>
+  </si>
+  <si>
+    <t>PWM X</t>
+  </si>
+  <si>
+    <t>sens X</t>
+  </si>
+  <si>
+    <t>Strat</t>
+  </si>
+  <si>
+    <t>QEA G</t>
+  </si>
+  <si>
+    <t>QEB G</t>
+  </si>
+  <si>
+    <t>QEA D</t>
+  </si>
+  <si>
+    <t>QEB D</t>
+  </si>
+  <si>
+    <t>PWM1L3</t>
+  </si>
+  <si>
+    <t>PWM1L2</t>
+  </si>
+  <si>
+    <t>PWM1H1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,7 +466,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -772,11 +830,117 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -784,142 +948,214 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -934,6 +1170,11 @@
       <color rgb="FFFFCCFF"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1012,6 +1253,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1046,6 +1288,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1221,615 +1464,615 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F36" sqref="A1:F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="13.5703125" style="1" customWidth="1"/>
     <col min="3" max="6" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>60</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="21" t="s">
+      <c r="F1" s="54"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="33"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="8" t="s">
+      <c r="E2" s="30"/>
+      <c r="F2" s="31"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="30" t="s">
+      <c r="C3" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="22" t="s">
+      <c r="E3" s="32"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="22" t="s">
+      <c r="C4" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="34"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="22" t="s">
+      <c r="E4" s="32"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="22" t="s">
+      <c r="C5" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
+      <c r="E5" s="32"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="22" t="s">
+      <c r="C6" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="22" t="s">
+      <c r="E6" s="32"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="22" t="s">
+      <c r="E7" s="32"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="22" t="s">
+      <c r="C8" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="34"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="22" t="s">
+      <c r="E8" s="32"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="22" t="s">
+      <c r="C9" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A10" s="42" t="s">
+      <c r="E9" s="32"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="37"/>
-      <c r="F10" s="38"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="45" t="s">
+      <c r="E10" s="35"/>
+      <c r="F10" s="36"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="46" t="s">
+      <c r="C11" s="42"/>
+      <c r="D11" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="33"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="8" t="s">
+      <c r="E11" s="30"/>
+      <c r="F11" s="31"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="30" t="s">
+      <c r="C12" s="25"/>
+      <c r="D12" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="34"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="22" t="s">
+      <c r="E12" s="32"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="34" t="s">
+      <c r="E13" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="22" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="22" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="22" t="s">
+      <c r="C15" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="8" t="s">
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" s="30" t="s">
+      <c r="C16" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="34"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="8" t="s">
+      <c r="E16" s="32"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="34"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="22" t="s">
+      <c r="E17" s="32"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="34"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="8" t="s">
+      <c r="E18" s="32"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="30" t="s">
+      <c r="C19" s="25"/>
+      <c r="D19" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="34"/>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="8" t="s">
+      <c r="E19" s="32"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="30" t="s">
+      <c r="C20" s="25"/>
+      <c r="D20" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="34"/>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="8" t="s">
+      <c r="E20" s="32"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="34"/>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="22" t="s">
+      <c r="E21" s="32"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="22" t="s">
+      <c r="D22" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="34"/>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="8" t="s">
+      <c r="E22" s="32"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="34"/>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="22" t="s">
+      <c r="E23" s="32"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="34"/>
-      <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="8" t="s">
+      <c r="E24" s="32"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="30" t="s">
+      <c r="C25" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="34"/>
-      <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A26" s="23" t="s">
+      <c r="E25" s="32"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="48" t="s">
+      <c r="C26" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="E26" s="35"/>
-      <c r="F26" s="6"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="40" t="s">
+      <c r="E26" s="33"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="D27" s="40" t="s">
+      <c r="C27" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="32" t="s">
+      <c r="E27" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F27" s="31" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="22" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D28" s="22" t="s">
+      <c r="C28" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E28" s="34" t="s">
+      <c r="E28" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="22" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" s="22" t="s">
+      <c r="C29" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="34" t="s">
+      <c r="E29" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="22" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30" s="22" t="s">
+      <c r="C30" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E30" s="34" t="s">
+      <c r="E30" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="F30" s="5"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="22" t="s">
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31" s="22" t="s">
+      <c r="C31" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="F31" s="5"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="22" t="s">
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="26" t="s">
+      <c r="C32" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="22" t="s">
+      <c r="D32" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E32" s="34"/>
-      <c r="F32" s="5"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="8" t="s">
+      <c r="E32" s="32"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="30" t="s">
+      <c r="C33" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="E33" s="34"/>
-      <c r="F33" s="5"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="8" t="s">
+      <c r="E33" s="32"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D34" s="30" t="s">
+      <c r="C34" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="E34" s="34"/>
-      <c r="F34" s="5"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="8" t="s">
+      <c r="E34" s="32"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35" s="30" t="s">
+      <c r="C35" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A36" s="23" t="s">
+      <c r="E35" s="32"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C36" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36" s="31" t="s">
+      <c r="C36" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="E36" s="35"/>
-      <c r="F36" s="6"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1841,24 +2084,621 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="55" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="54"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="30"/>
+      <c r="F2" s="31"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="32"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="32"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="32"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="32"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="32"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="57" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="32"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="70" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="35"/>
+      <c r="F10" s="36"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="64"/>
+      <c r="D11" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="30"/>
+      <c r="F11" s="31"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="65"/>
+      <c r="D12" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="32"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="32"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="32"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="68" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="68" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="32"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="32"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="65"/>
+      <c r="D19" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="32"/>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="65"/>
+      <c r="D20" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="32"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="32"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="62" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" s="32"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="32"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" s="32"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" s="32"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="63" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="72" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="69" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="33"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="59" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="71" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="32"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33" s="32"/>
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="32"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E35" s="32"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" s="33"/>
+      <c r="F36" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>